<commit_message>
Update on monitoring report
Data collection monitoring report both in html and pdf.
</commit_message>
<xml_diff>
--- a/input/sample/Final_sampling_frame_EJ_95_9_CS 5_B 15.xlsx
+++ b/input/sample/Final_sampling_frame_EJ_95_9_CS 5_B 15.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evelyn GAKINYA\Documents\2. Data cleaning\data cleaning scripts\input\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evelyn GAKINYA\Documents\2. Data cleaning\MSNA_Data_Cleaning_Opt\input\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="52">
   <si>
     <t>id_sampl</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>East Jerusalem</t>
+  </si>
+  <si>
+    <t>strata</t>
+  </si>
+  <si>
+    <t>East_Jerusalem</t>
   </si>
 </sst>
 </file>
@@ -993,15 +999,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1044,8 +1050,11 @@
       <c r="N1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1088,8 +1097,11 @@
       <c r="N2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1132,8 +1144,11 @@
       <c r="N3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1176,8 +1191,11 @@
       <c r="N4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1220,8 +1238,11 @@
       <c r="N5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1264,8 +1285,11 @@
       <c r="N6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1308,8 +1332,11 @@
       <c r="N7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1352,8 +1379,11 @@
       <c r="N8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1396,8 +1426,11 @@
       <c r="N9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1440,8 +1473,11 @@
       <c r="N10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1484,8 +1520,11 @@
       <c r="N11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1528,8 +1567,11 @@
       <c r="N12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1572,8 +1614,11 @@
       <c r="N13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1616,8 +1661,11 @@
       <c r="N14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1660,8 +1708,11 @@
       <c r="N15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1704,8 +1755,11 @@
       <c r="N16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1748,8 +1802,11 @@
       <c r="N17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1792,8 +1849,11 @@
       <c r="N18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1836,8 +1896,11 @@
       <c r="N19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1880,8 +1943,11 @@
       <c r="N20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1924,8 +1990,11 @@
       <c r="N21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1968,8 +2037,11 @@
       <c r="N22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2012,8 +2084,11 @@
       <c r="N23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2056,8 +2131,11 @@
       <c r="N24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2100,8 +2178,11 @@
       <c r="N25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2144,8 +2225,11 @@
       <c r="N26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2188,8 +2272,11 @@
       <c r="N27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2232,8 +2319,11 @@
       <c r="N28" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2276,8 +2366,11 @@
       <c r="N29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2320,8 +2413,11 @@
       <c r="N30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2364,8 +2460,11 @@
       <c r="N31" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2408,8 +2507,11 @@
       <c r="N32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2452,8 +2554,11 @@
       <c r="N33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2496,8 +2601,11 @@
       <c r="N34" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2539,6 +2647,9 @@
       </c>
       <c r="N35" t="s">
         <v>49</v>
+      </c>
+      <c r="O35" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>